<commit_message>
added references for cost tables
</commit_message>
<xml_diff>
--- a/paper_graphics/data/changes_costs_assumptions.xlsx
+++ b/paper_graphics/data/changes_costs_assumptions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marta\Dropbox\AU\TRANSITION_ WORKING\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au595690\Dropbox\AU\TRANSITION PATHS\transition_paths_paper\paper_graphics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="5805"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="5805" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="cost generators" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="fuel_costs" sheetId="2" r:id="rId3"/>
     <sheet name="emissions" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -146,9 +146,6 @@
     <t>https://www.eia.gov/energyexplained/coal/prices-and-outlook.php</t>
   </si>
   <si>
-    <t>BP 2019 Approximate conversin factors</t>
-  </si>
-  <si>
     <t>€/MWh</t>
   </si>
   <si>
@@ -435,12 +432,15 @@
   </si>
   <si>
     <t>JRC</t>
+  </si>
+  <si>
+    <t>BP 2019 Approximate conversion factors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -448,7 +448,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -483,6 +483,13 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -576,7 +583,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -653,6 +660,7 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -677,7 +685,7 @@
     <xf numFmtId="4" fontId="4" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Body: normal cell" xfId="2"/>
@@ -819,16 +827,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>145538</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>69338</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>276225</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -852,7 +860,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7543800" y="1117088"/>
+          <a:off x="9401175" y="1240913"/>
           <a:ext cx="3295650" cy="1616587"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -876,7 +884,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1140,11 +1148,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G80" sqref="G80"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.140625" customWidth="1"/>
@@ -1214,7 +1222,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="9">
         <f>(3.5+4.25)/2*$G$2</f>
@@ -1303,7 +1311,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="9">
         <f>(2.75+5)/2*$G$2</f>
@@ -1404,7 +1412,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="9">
         <f>C13</f>
@@ -1456,7 +1464,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="6">
-        <v>600</v>
+        <v>454</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>9</v>
@@ -1467,8 +1475,8 @@
         <v>5</v>
       </c>
       <c r="C28" s="7">
-        <f>20000/(0.6*1000000)</f>
-        <v>3.3333333333333333E-2</v>
+        <f>8068/(0.454*1000000)</f>
+        <v>1.777092511013216E-2</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>9</v>
@@ -1476,7 +1484,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="8">
         <v>4.5</v>
@@ -1490,7 +1498,7 @@
         <v>10</v>
       </c>
       <c r="C30" s="8">
-        <v>0.39</v>
+        <v>0.4</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>9</v>
@@ -1791,7 +1799,7 @@
         <v>30</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F50" t="s">
         <v>0</v>
@@ -1820,7 +1828,7 @@
         <v>1150</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F51" t="s">
         <v>23</v>
@@ -1850,7 +1858,7 @@
         <v>800</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F52" t="s">
         <v>24</v>
@@ -1880,7 +1888,7 @@
         <v>550</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F53" t="s">
         <v>28</v>
@@ -1906,7 +1914,7 @@
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>0</v>
@@ -1946,7 +1954,7 @@
         <v>10</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D58" s="10"/>
     </row>
@@ -1968,7 +1976,7 @@
     </row>
     <row r="61" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>0</v>
@@ -1980,7 +1988,7 @@
         <v>9</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F61" s="10" t="s">
         <v>0</v>
@@ -1992,7 +2000,7 @@
         <v>9</v>
       </c>
       <c r="I61" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J61" s="10" t="s">
         <v>0</v>
@@ -2004,7 +2012,7 @@
         <v>9</v>
       </c>
       <c r="M61" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N61" s="10" t="s">
         <v>0</v>
@@ -2015,16 +2023,16 @@
       <c r="P61" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="Q61" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="R61" s="38"/>
-      <c r="S61" s="38"/>
-      <c r="T61" s="38"/>
+      <c r="Q61" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="R61" s="39"/>
+      <c r="S61" s="39"/>
+      <c r="T61" s="39"/>
     </row>
     <row r="62" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B62" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C62" s="6">
         <v>3500</v>
@@ -2033,7 +2041,7 @@
         <v>9</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G62" s="10">
         <v>2300</v>
@@ -2042,7 +2050,7 @@
         <v>9</v>
       </c>
       <c r="J62" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K62" s="10">
         <v>3400</v>
@@ -2051,7 +2059,7 @@
         <v>9</v>
       </c>
       <c r="N62" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O62" s="10">
         <v>7800</v>
@@ -2062,28 +2070,28 @@
     </row>
     <row r="63" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C63" s="6">
         <v>1070</v>
       </c>
       <c r="D63" s="6"/>
       <c r="F63" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G63" s="10">
         <v>750</v>
       </c>
       <c r="H63" s="10"/>
       <c r="J63" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K63" s="10">
         <v>1000</v>
       </c>
       <c r="L63" s="10"/>
       <c r="N63" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O63" s="10">
         <v>1830</v>
@@ -2134,14 +2142,14 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B65" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C65" s="9">
         <v>1.9</v>
       </c>
       <c r="D65" s="6"/>
       <c r="F65" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G65" s="11">
         <v>1.6</v>
@@ -2150,7 +2158,7 @@
         <v>9</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K65" s="11">
         <v>3.8</v>
@@ -2159,7 +2167,7 @@
         <v>9</v>
       </c>
       <c r="N65" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O65" s="11">
         <v>24.8</v>
@@ -2173,34 +2181,34 @@
         <v>10</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D66" s="6"/>
       <c r="F66" s="10" t="s">
         <v>10</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H66" s="10"/>
       <c r="J66" s="10" t="s">
         <v>10</v>
       </c>
       <c r="K66" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L66" s="10"/>
       <c r="N66" s="10" t="s">
         <v>10</v>
       </c>
       <c r="O66" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P66" s="10"/>
     </row>
     <row r="67" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C67" s="17">
         <v>0.29299999999999998</v>
@@ -2209,7 +2217,7 @@
         <v>9</v>
       </c>
       <c r="F67" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G67" s="15">
         <v>0.31</v>
@@ -2218,7 +2226,7 @@
         <v>9</v>
       </c>
       <c r="J67" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K67" s="15">
         <v>0.28000000000000003</v>
@@ -2227,7 +2235,7 @@
         <v>9</v>
       </c>
       <c r="N67" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O67" s="15">
         <v>0.221</v>
@@ -2238,14 +2246,14 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B68" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C68" s="9">
         <f>fuel_costs!$F$3</f>
         <v>25.2</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F68" s="14"/>
       <c r="G68" s="15"/>
@@ -2273,7 +2281,7 @@
     </row>
     <row r="70" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>0</v>
@@ -2285,7 +2293,7 @@
         <v>9</v>
       </c>
       <c r="E70" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F70" s="10" t="s">
         <v>0</v>
@@ -2297,7 +2305,7 @@
         <v>9</v>
       </c>
       <c r="I70" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J70" s="10" t="s">
         <v>0</v>
@@ -2311,7 +2319,7 @@
     </row>
     <row r="71" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="B71" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C71" s="6">
         <v>890</v>
@@ -2320,7 +2328,7 @@
         <v>9</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G71">
         <v>720</v>
@@ -2329,7 +2337,7 @@
         <v>9</v>
       </c>
       <c r="J71" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K71">
         <v>648</v>
@@ -2340,21 +2348,21 @@
     </row>
     <row r="72" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B72" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C72" s="19">
         <v>900</v>
       </c>
       <c r="D72" s="6"/>
       <c r="F72" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G72" s="18">
         <v>720</v>
       </c>
       <c r="H72" s="10"/>
       <c r="J72" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K72" s="18">
         <v>790</v>
@@ -2395,7 +2403,7 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B74" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C74" s="8">
         <v>0.6</v>
@@ -2404,7 +2412,7 @@
         <v>9</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G74" s="11">
         <v>0.5</v>
@@ -2413,7 +2421,7 @@
         <v>9</v>
       </c>
       <c r="J74" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K74" s="11">
         <v>1</v>
@@ -2453,14 +2461,14 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B76" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C76" s="9">
         <f>fuel_costs!$F$3</f>
         <v>25.2</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J76" s="14"/>
     </row>
@@ -2469,22 +2477,22 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B78" s="6">
         <v>2030</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D78" s="6">
         <v>25.2</v>
       </c>
       <c r="E78" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F78" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2505,7 +2513,7 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
@@ -2516,7 +2524,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -2539,7 +2547,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" s="6">
         <v>132</v>
@@ -2548,7 +2556,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G2">
         <f>192*0.9</f>
@@ -2581,7 +2589,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="6">
         <v>270</v>
@@ -2590,7 +2598,7 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G4">
         <f>411*0.9</f>
@@ -2646,12 +2654,12 @@
         <v>28600</v>
       </c>
       <c r="H7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G8">
         <v>33.33</v>
@@ -2659,7 +2667,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G9">
         <f>C23</f>
@@ -2668,7 +2676,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G10" s="2">
         <f>G8/G9</f>
@@ -2686,14 +2694,14 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G12">
         <f>30.7*1000000</f>
         <v>30700000</v>
       </c>
       <c r="H12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2716,38 +2724,38 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C16">
         <v>350</v>
       </c>
       <c r="D16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C17">
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C18">
         <v>0.8</v>
       </c>
       <c r="D18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2758,43 +2766,43 @@
         <v>0.04</v>
       </c>
       <c r="D19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C21">
         <v>339</v>
       </c>
       <c r="D21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C22">
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C23">
         <v>0.57999999999999996</v>
       </c>
       <c r="D23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2805,7 +2813,7 @@
         <v>0.03</v>
       </c>
       <c r="D24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2819,10 +2827,10 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
@@ -2834,7 +2842,7 @@
         <v>31</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2849,9 +2857,9 @@
         <v>30</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="46">
+        <v>39</v>
+      </c>
+      <c r="F2" s="38">
         <v>7</v>
       </c>
       <c r="G2" s="10"/>
@@ -2864,13 +2872,13 @@
         <v>3412141.4798968998</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" s="6">
         <v>25.2</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2890,25 +2898,25 @@
         <v>0.9</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F5" s="10">
         <v>7</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2">
         <f>B4*B5</f>
         <v>20.10843216932841</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F6" s="10">
         <v>0.28000000000000003</v>
@@ -2917,9 +2925,9 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="46">
+        <v>39</v>
+      </c>
+      <c r="F7" s="38">
         <f>F5/F6</f>
         <v>24.999999999999996</v>
       </c>
@@ -2969,7 +2977,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="2">
         <f>B11*B12</f>
@@ -2998,7 +3006,7 @@
         <v>4.0705</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3020,7 +3028,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="2">
         <f>B18*B19</f>
@@ -3042,11 +3050,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -3629,37 +3637,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
+      <c r="A1" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" s="21"/>
       <c r="F2" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H2" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="M2">
         <v>2.9307099999999999E-7</v>
@@ -3667,53 +3675,53 @@
     </row>
     <row r="3" spans="1:13" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="25" t="s">
         <v>70</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>71</v>
       </c>
       <c r="C3" s="25"/>
       <c r="D3" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" s="27" t="s">
+    </row>
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="44" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="28">
         <v>12.7</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" s="28">
         <f t="shared" ref="D5:D13" si="0">B5/2.20462</f>
         <v>5.7606299498326248</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F5" s="28">
         <v>139.04859867504859</v>
@@ -3725,20 +3733,20 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" s="28">
         <v>14.8</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D6" s="28">
         <f t="shared" si="0"/>
         <v>6.7131750596474689</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F6" s="28">
         <v>143.19829002512873</v>
@@ -3750,20 +3758,20 @@
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" s="28">
         <v>13.7</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="28">
         <f t="shared" si="0"/>
         <v>6.214222859268264</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="28">
         <v>141.12344435008868</v>
@@ -3775,20 +3783,20 @@
     </row>
     <row r="8" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="28">
         <v>22.4</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" s="28">
         <f t="shared" si="0"/>
         <v>10.160481171358329</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8" s="28">
         <v>161.30000000000001</v>
@@ -3800,20 +3808,20 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="28">
         <v>21.5</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="28">
         <f t="shared" si="0"/>
         <v>9.7522475528662547</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F9" s="28">
         <v>159.4</v>
@@ -3826,20 +3834,20 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="28">
         <v>4631.5</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D10" s="28">
         <f t="shared" si="0"/>
         <v>2100.8155600511654</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F10" s="28">
         <v>210.2</v>
@@ -3855,20 +3863,20 @@
     </row>
     <row r="11" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="28">
         <v>117.1</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="28">
         <f t="shared" si="0"/>
         <v>53.115729694913412</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F11" s="28">
         <v>117</v>
@@ -3881,23 +3889,26 @@
         <f>(G11/1000)*($M$2*1000000)</f>
         <v>1.5553386524661846E-2</v>
       </c>
+      <c r="I11" s="47">
+        <v>0.187</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B12" s="28">
         <v>19.600000000000001</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="28">
         <f t="shared" si="0"/>
         <v>8.89042102493854</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F12" s="28">
         <v>157.19999999999999</v>
@@ -3908,20 +3919,20 @@
     </row>
     <row r="13" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B13" s="28">
         <v>26</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D13" s="28">
         <f t="shared" si="0"/>
         <v>11.793415645326633</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F13" s="28">
         <v>173.7</v>
@@ -3932,32 +3943,32 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
+      <c r="A14" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" s="28">
         <v>21.1</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15" s="28">
         <f>B15/2.20462</f>
         <v>9.5708103890919993</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F15" s="28">
         <v>156.30000000000001</v>
@@ -3969,20 +3980,20 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B16" s="28">
         <v>18.399999999999999</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" s="28">
         <f>B16/2.20462</f>
         <v>8.3461095336157705</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F16" s="28">
         <v>152.6</v>
@@ -3991,33 +4002,33 @@
         <v>69.2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+    </row>
+    <row r="18" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
         <v>90</v>
-      </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-    </row>
-    <row r="18" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
-        <v>91</v>
       </c>
       <c r="B18" s="28">
         <v>120.7</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D18" s="28">
         <f>B18/2.20462</f>
         <v>54.748664168881717</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F18" s="28">
         <v>120.6</v>
@@ -4027,22 +4038,22 @@
         <v>54.703304877938152</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B19" s="28">
         <v>32.4</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D19" s="28">
         <f>B19/2.20462</f>
         <v>14.696410265714727</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F19" s="28">
         <v>225.1</v>
@@ -4052,23 +4063,23 @@
         <v>102.10376391396251</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" s="28">
         <f>F20*5.796/42</f>
         <v>22.093800000000002</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D20" s="28">
         <f>B20/2.20462</f>
         <v>10.021591022489138</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F20" s="28">
         <v>160.1</v>
@@ -4078,34 +4089,34 @@
         <v>72.620224800645914</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
         <v>94</v>
-      </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
-        <v>95</v>
       </c>
       <c r="B22" s="28">
         <f>F22*6.636/42</f>
         <v>26.3386</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D22" s="28">
         <f>B22/2.20462</f>
         <v>11.94700220446154</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F22" s="28">
         <v>166.7</v>
@@ -4115,23 +4126,23 @@
         <v>75.613938002921145</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" s="28">
         <f>F23*6.065/42</f>
         <v>23.624619047619049</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D23" s="28">
         <f>B23/2.20462</f>
         <v>10.715959688118158</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F23" s="28">
         <v>163.6</v>
@@ -4141,23 +4152,23 @@
         <v>74.207799983670654</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" s="28">
         <f>F24*6.636/42</f>
         <v>24.742799999999999</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" s="28">
         <f>B24/2.20462</f>
         <v>11.223158639584147</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F24" s="28">
         <v>156.6</v>
@@ -4167,23 +4178,23 @@
         <v>71.032649617621175</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B25" s="28">
         <f>F25*5.248/42</f>
         <v>20.054857142857145</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D25" s="28">
         <f>B25/2.20462</f>
         <v>9.0967409997446946</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F25" s="28">
         <v>160.5</v>
@@ -4193,23 +4204,23 @@
         <v>72.801661964420177</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B26" s="28">
         <f>F26*5.537/42</f>
         <v>21.106516666666668</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D26" s="28">
         <f>B26/2.20462</f>
         <v>9.5737663028851543</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F26" s="28">
         <v>160.1</v>
@@ -4219,33 +4230,33 @@
         <v>72.620224800645914</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="45" t="s">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="29" t="s">
         <v>100</v>
-      </c>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
-        <v>101</v>
       </c>
       <c r="B28" s="28">
         <v>5685</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D28" s="28">
         <f>B28/2.20462</f>
         <v>2578.675690141612</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F28" s="28">
         <v>228.6</v>
@@ -4257,23 +4268,26 @@
         <f>(G28/1000)*($M$2*1000000)</f>
         <v>3.0391462699999996E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="47">
+        <v>0.35399999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B29" s="28">
         <v>4931.3</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D29" s="28">
         <f>B29/2.20462</f>
         <v>2236.8027142999704</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F29" s="28">
         <v>205.7</v>
@@ -4286,22 +4300,22 @@
         <v>2.7343524299999995E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B30" s="28">
         <v>3715.9</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D30" s="28">
         <f>B30/2.20462</f>
         <v>1685.5058921718937</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F30" s="28">
         <v>214.3</v>
@@ -4314,7 +4328,7 @@
         <v>2.84865012E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
         <v>7</v>
       </c>
@@ -4322,14 +4336,14 @@
         <v>2791.6</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D31" s="28">
         <f>B31/2.20462</f>
         <v>1266.2499659805319</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F31" s="28">
         <v>215.4</v>
@@ -4342,24 +4356,27 @@
         <f>(G31/1000)*($M$2*1000000)</f>
         <v>2.8634183396685144E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="47">
+        <v>0.33400000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B32" s="30">
         <f>F32*24.8</f>
         <v>6239.68</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D32" s="30">
         <f>B32/2.20462</f>
         <v>2830.2746051473728</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F32" s="30">
         <v>251.6</v>
@@ -4371,7 +4388,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B33" s="30"/>
       <c r="C33" s="30"/>
@@ -4382,14 +4399,14 @@
     </row>
     <row r="34" spans="1:7" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="32" t="s">
         <v>106</v>
-      </c>
-      <c r="B34" s="32" t="s">
-        <v>107</v>
       </c>
       <c r="C34" s="32"/>
       <c r="D34" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E34" s="30"/>
       <c r="F34" s="30">
@@ -4402,20 +4419,20 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B35" s="30">
         <v>5771</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D35" s="30">
         <f>B35/2.20462</f>
         <v>2617.6846803530771</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F35" s="30">
         <v>91.9</v>
@@ -4427,20 +4444,20 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B36" s="30">
         <v>6160</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D36" s="30">
         <f>B36/2.20462</f>
         <v>2794.1323221235407</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F36" s="30">
         <v>189.54</v>
@@ -4452,21 +4469,21 @@
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B37" s="33">
         <f>F37*4.4</f>
         <v>924.00000000000011</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D37" s="30">
         <f>B37/2.20462</f>
         <v>419.11984831853118</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F37" s="34">
         <v>210</v>
@@ -4477,46 +4494,46 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+    </row>
+    <row r="39" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B38" s="39"/>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-    </row>
-    <row r="39" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="40" t="s">
+      <c r="B39" s="41"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="41"/>
+    </row>
+    <row r="40" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="B39" s="40"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="40"/>
-      <c r="F39" s="40"/>
-      <c r="G39" s="40"/>
-    </row>
-    <row r="40" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="40"/>
-      <c r="G40" s="40"/>
+      <c r="B40" s="41"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="41"/>
+      <c r="G40" s="41"/>
     </row>
     <row r="41" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
       <c r="C41" s="20"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="41"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
     </row>
     <row r="42" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20"/>

</xml_diff>

<commit_message>
small changes in tables
</commit_message>
<xml_diff>
--- a/paper_graphics/data/changes_costs_assumptions.xlsx
+++ b/paper_graphics/data/changes_costs_assumptions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="5805" activeTab="3"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="cost generators" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="137">
   <si>
     <t>Lifetime</t>
   </si>
@@ -435,6 +443,9 @@
   </si>
   <si>
     <t>BP 2019 Approximate conversion factors</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -583,7 +594,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -661,6 +672,8 @@
     <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -685,7 +698,6 @@
     <xf numFmtId="4" fontId="4" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Body: normal cell" xfId="2"/>
@@ -725,7 +737,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -780,7 +798,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -802,66 +826,6 @@
         <a:xfrm>
           <a:off x="11639550" y="9214446"/>
           <a:ext cx="3181349" cy="2266639"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>69338</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9401175" y="1240913"/>
-          <a:ext cx="3295650" cy="1616587"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1148,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T78"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2023,19 +1987,19 @@
       <c r="P61" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="Q61" s="39" t="s">
+      <c r="Q61" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="R61" s="39"/>
-      <c r="S61" s="39"/>
-      <c r="T61" s="39"/>
+      <c r="R61" s="41"/>
+      <c r="S61" s="41"/>
+      <c r="T61" s="41"/>
     </row>
     <row r="62" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B62" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C62" s="6">
-        <v>3500</v>
+      <c r="C62" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>9</v>
@@ -3050,8 +3014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3637,15 +3601,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
@@ -3696,15 +3660,15 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
@@ -3889,9 +3853,11 @@
         <f>(G11/1000)*($M$2*1000000)</f>
         <v>1.5553386524661846E-2</v>
       </c>
-      <c r="I11" s="47">
-        <v>0.187</v>
-      </c>
+      <c r="I11" s="40">
+        <f>(G11/1000)/($M$2*1000000)</f>
+        <v>0.18108366369913725</v>
+      </c>
+      <c r="J11" s="39"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
@@ -3943,15 +3909,15 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
@@ -4003,15 +3969,15 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
     </row>
     <row r="18" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
@@ -4090,15 +4056,15 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
@@ -4231,15 +4197,15 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="B27" s="46"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="46"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
@@ -4268,8 +4234,9 @@
         <f>(G28/1000)*($M$2*1000000)</f>
         <v>3.0391462699999996E-2</v>
       </c>
-      <c r="I28" s="47">
-        <v>0.35399999999999998</v>
+      <c r="I28" s="40">
+        <f>(G28/1000)/($M$2*1000000)</f>
+        <v>0.35383917207775595</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -4356,7 +4323,7 @@
         <f>(G31/1000)*($M$2*1000000)</f>
         <v>2.8634183396685144E-2</v>
       </c>
-      <c r="I31" s="47">
+      <c r="I31" s="39">
         <v>0.33400000000000002</v>
       </c>
     </row>
@@ -4494,46 +4461,46 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="40" t="s">
+      <c r="A38" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="40"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="40"/>
-      <c r="G38" s="40"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42"/>
     </row>
     <row r="39" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="41" t="s">
+      <c r="A39" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="B39" s="41"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="41"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
     </row>
     <row r="40" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="41" t="s">
+      <c r="A40" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="B40" s="41"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="41"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
     </row>
     <row r="41" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
       <c r="C41" s="20"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="44"/>
     </row>
     <row r="42" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20"/>
@@ -4565,6 +4532,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added battery to balancing in Figure 2
</commit_message>
<xml_diff>
--- a/paper_graphics/data/changes_costs_assumptions.xlsx
+++ b/paper_graphics/data/changes_costs_assumptions.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="cost generators" sheetId="1" r:id="rId1"/>
     <sheet name="cost storage" sheetId="4" r:id="rId2"/>
     <sheet name="fuel_costs" sheetId="2" r:id="rId3"/>
     <sheet name="emissions" sheetId="3" r:id="rId4"/>
+    <sheet name="PV_cost_evolution_DEA" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="147">
   <si>
     <t>Lifetime</t>
   </si>
@@ -163,15 +164,6 @@
     <t>ETIP 2019</t>
   </si>
   <si>
-    <t>ETIP 2020</t>
-  </si>
-  <si>
-    <t>ETIP 2021</t>
-  </si>
-  <si>
-    <t>ETIP 2022</t>
-  </si>
-  <si>
     <t>CHP coal</t>
   </si>
   <si>
@@ -476,20 +468,30 @@
   </si>
   <si>
     <t>* It seems to be an error in DEA database so we keep using previous assumptions</t>
+  </si>
+  <si>
+    <t>FOM (%)</t>
+  </si>
+  <si>
+    <t>large power plants DEA</t>
+  </si>
+  <si>
+    <t>small isntallations DEA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,6 +537,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -550,7 +565,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -605,6 +620,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -624,7 +691,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -728,6 +795,33 @@
     <xf numFmtId="4" fontId="4" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Body: normal cell" xfId="2"/>
@@ -1202,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T78"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,7 +1370,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C5" s="9">
         <f>(3.5+4.25)/2*$G$2</f>
@@ -1365,7 +1459,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C13" s="9">
         <f>(2.75+5)/2*$G$2</f>
@@ -1466,7 +1560,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C22" s="9">
         <f>C13</f>
@@ -1538,7 +1632,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C29" s="8">
         <v>4.5</v>
@@ -1882,7 +1976,7 @@
         <v>1150</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F51" t="s">
         <v>23</v>
@@ -1912,7 +2006,7 @@
         <v>800</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F52" t="s">
         <v>24</v>
@@ -1942,7 +2036,7 @@
         <v>550</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F53" t="s">
         <v>28</v>
@@ -1968,7 +2062,7 @@
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>0</v>
@@ -2008,7 +2102,7 @@
         <v>10</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D58" s="10"/>
     </row>
@@ -2030,7 +2124,7 @@
     </row>
     <row r="61" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>0</v>
@@ -2042,7 +2136,7 @@
         <v>9</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F61" s="10" t="s">
         <v>0</v>
@@ -2054,7 +2148,7 @@
         <v>9</v>
       </c>
       <c r="I61" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J61" s="10" t="s">
         <v>0</v>
@@ -2066,7 +2160,7 @@
         <v>9</v>
       </c>
       <c r="M61" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="N61" s="10" t="s">
         <v>0</v>
@@ -2078,7 +2172,7 @@
         <v>9</v>
       </c>
       <c r="Q61" s="41" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="R61" s="41"/>
       <c r="S61" s="41"/>
@@ -2086,16 +2180,16 @@
     </row>
     <row r="62" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B62" s="16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G62" s="10">
         <v>2300</v>
@@ -2104,7 +2198,7 @@
         <v>9</v>
       </c>
       <c r="J62" s="14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K62" s="10">
         <v>3400</v>
@@ -2113,7 +2207,7 @@
         <v>9</v>
       </c>
       <c r="N62" s="14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="O62" s="10">
         <v>7800</v>
@@ -2124,28 +2218,28 @@
     </row>
     <row r="63" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C63" s="6">
         <v>1070</v>
       </c>
       <c r="D63" s="6"/>
       <c r="F63" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G63" s="10">
         <v>750</v>
       </c>
       <c r="H63" s="10"/>
       <c r="J63" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K63" s="10">
         <v>1000</v>
       </c>
       <c r="L63" s="10"/>
       <c r="N63" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="O63" s="10">
         <v>1830</v>
@@ -2196,14 +2290,14 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B65" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C65" s="9">
         <v>1.9</v>
       </c>
       <c r="D65" s="6"/>
       <c r="F65" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G65" s="11">
         <v>1.6</v>
@@ -2212,7 +2306,7 @@
         <v>9</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K65" s="11">
         <v>3.8</v>
@@ -2221,7 +2315,7 @@
         <v>9</v>
       </c>
       <c r="N65" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="O65" s="11">
         <v>24.8</v>
@@ -2235,34 +2329,34 @@
         <v>10</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D66" s="6"/>
       <c r="F66" s="10" t="s">
         <v>10</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H66" s="10"/>
       <c r="J66" s="10" t="s">
         <v>10</v>
       </c>
       <c r="K66" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L66" s="10"/>
       <c r="N66" s="10" t="s">
         <v>10</v>
       </c>
       <c r="O66" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="P66" s="10"/>
     </row>
     <row r="67" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C67" s="17">
         <v>0.29299999999999998</v>
@@ -2271,7 +2365,7 @@
         <v>9</v>
       </c>
       <c r="F67" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G67" s="15">
         <v>0.31</v>
@@ -2280,7 +2374,7 @@
         <v>9</v>
       </c>
       <c r="J67" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K67" s="15">
         <v>0.28000000000000003</v>
@@ -2289,7 +2383,7 @@
         <v>9</v>
       </c>
       <c r="N67" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O67" s="15">
         <v>0.221</v>
@@ -2300,14 +2394,14 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B68" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C68" s="9">
         <f>fuel_costs!$F$3</f>
         <v>25.2</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F68" s="14"/>
       <c r="G68" s="15"/>
@@ -2335,7 +2429,7 @@
     </row>
     <row r="70" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>0</v>
@@ -2347,7 +2441,7 @@
         <v>9</v>
       </c>
       <c r="E70" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F70" s="10" t="s">
         <v>0</v>
@@ -2359,7 +2453,7 @@
         <v>9</v>
       </c>
       <c r="I70" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J70" s="10" t="s">
         <v>0</v>
@@ -2373,7 +2467,7 @@
     </row>
     <row r="71" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="B71" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C71" s="6">
         <v>890</v>
@@ -2382,7 +2476,7 @@
         <v>9</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G71">
         <v>720</v>
@@ -2391,7 +2485,7 @@
         <v>9</v>
       </c>
       <c r="J71" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K71">
         <v>648</v>
@@ -2402,21 +2496,21 @@
     </row>
     <row r="72" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B72" s="16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C72" s="19">
         <v>900</v>
       </c>
       <c r="D72" s="6"/>
       <c r="F72" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G72" s="18">
         <v>720</v>
       </c>
       <c r="H72" s="10"/>
       <c r="J72" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K72" s="18">
         <v>790</v>
@@ -2457,7 +2551,7 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B74" s="16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C74" s="8">
         <v>0.6</v>
@@ -2466,7 +2560,7 @@
         <v>9</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G74" s="11">
         <v>0.5</v>
@@ -2475,7 +2569,7 @@
         <v>9</v>
       </c>
       <c r="J74" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K74" s="11">
         <v>1</v>
@@ -2515,14 +2609,14 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B76" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C76" s="9">
         <f>fuel_costs!$F$3</f>
         <v>25.2</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J76" s="14"/>
     </row>
@@ -2531,22 +2625,22 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B78" s="6">
         <v>2030</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D78" s="6">
         <v>25.2</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2563,7 +2657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
@@ -2581,7 +2675,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -2604,7 +2698,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C2" s="6">
         <v>132</v>
@@ -2613,7 +2707,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G2">
         <f>192*0.9</f>
@@ -2646,7 +2740,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C4" s="6">
         <v>270</v>
@@ -2655,7 +2749,7 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G4">
         <f>411*0.9</f>
@@ -2711,10 +2805,10 @@
         <v>28600</v>
       </c>
       <c r="H7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J7" s="10" t="s">
         <v>20</v>
@@ -2726,18 +2820,18 @@
         <v>9</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G8">
         <v>33.33</v>
       </c>
       <c r="I8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="J8" s="10" t="s">
         <v>20</v>
@@ -2749,12 +2843,12 @@
         <v>9</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G9">
         <f>C23</f>
@@ -2763,7 +2857,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G10" s="2">
         <f>G8/G9</f>
@@ -2788,7 +2882,7 @@
         <v>30700000</v>
       </c>
       <c r="H12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2811,22 +2905,22 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B16" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C16">
         <v>350</v>
       </c>
       <c r="D16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="K16">
         <v>0.57999999999999996</v>
@@ -2837,13 +2931,13 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C17">
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J17" s="10" t="s">
         <v>20</v>
@@ -2858,13 +2952,13 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C18">
         <v>0.8</v>
       </c>
       <c r="D18" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -2875,13 +2969,13 @@
         <v>0.04</v>
       </c>
       <c r="D19" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I19" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="K19">
         <v>30</v>
@@ -2889,7 +2983,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J20" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="K20">
         <v>46.8</v>
@@ -2897,16 +2991,16 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B21" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C21">
         <v>339</v>
       </c>
       <c r="D21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J21" t="s">
         <v>20</v>
@@ -2918,24 +3012,24 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C22">
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C23">
         <v>0.57999999999999996</v>
       </c>
       <c r="D23" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -2946,10 +3040,10 @@
         <v>0.03</v>
       </c>
       <c r="D24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J24" s="10" t="s">
         <v>20</v>
@@ -2961,15 +3055,15 @@
         <v>9</v>
       </c>
       <c r="M24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I26" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J26" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="K26">
         <v>860</v>
@@ -2977,7 +3071,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J27" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="K27">
         <v>46.8</v>
@@ -3019,7 +3113,7 @@
         <v>31</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3055,7 +3149,7 @@
         <v>25.2</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3075,13 +3169,13 @@
         <v>0.9</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F5" s="10">
         <v>7</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -3093,7 +3187,7 @@
         <v>20.10843216932841</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F6" s="10">
         <v>0.28000000000000003</v>
@@ -3183,7 +3277,7 @@
         <v>4.0705</v>
       </c>
       <c r="C17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3815,7 +3909,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -3827,24 +3921,24 @@
     <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E2" s="21"/>
       <c r="F2" s="22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="M2">
         <v>2.9307099999999999E-7</v>
@@ -3852,29 +3946,29 @@
     </row>
     <row r="3" spans="1:13" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C3" s="25"/>
       <c r="D3" s="25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B4" s="46"/>
       <c r="C4" s="46"/>
@@ -3885,20 +3979,20 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B5" s="28">
         <v>12.7</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D5" s="28">
         <f t="shared" ref="D5:D13" si="0">B5/2.20462</f>
         <v>5.7606299498326248</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F5" s="28">
         <v>139.04859867504859</v>
@@ -3910,20 +4004,20 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B6" s="28">
         <v>14.8</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D6" s="28">
         <f t="shared" si="0"/>
         <v>6.7131750596474689</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F6" s="28">
         <v>143.19829002512873</v>
@@ -3935,20 +4029,20 @@
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B7" s="28">
         <v>13.7</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D7" s="28">
         <f t="shared" si="0"/>
         <v>6.214222859268264</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F7" s="28">
         <v>141.12344435008868</v>
@@ -3960,20 +4054,20 @@
     </row>
     <row r="8" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" s="28">
         <v>22.4</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D8" s="28">
         <f t="shared" si="0"/>
         <v>10.160481171358329</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F8" s="28">
         <v>161.30000000000001</v>
@@ -3985,20 +4079,20 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B9" s="28">
         <v>21.5</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D9" s="28">
         <f t="shared" si="0"/>
         <v>9.7522475528662547</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F9" s="28">
         <v>159.4</v>
@@ -4011,20 +4105,20 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B10" s="28">
         <v>4631.5</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D10" s="28">
         <f t="shared" si="0"/>
         <v>2100.8155600511654</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F10" s="28">
         <v>210.2</v>
@@ -4040,20 +4134,20 @@
     </row>
     <row r="11" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B11" s="28">
         <v>117.1</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D11" s="28">
         <f t="shared" si="0"/>
         <v>53.115729694913412</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F11" s="28">
         <v>117</v>
@@ -4074,20 +4168,20 @@
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B12" s="28">
         <v>19.600000000000001</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D12" s="28">
         <f t="shared" si="0"/>
         <v>8.89042102493854</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F12" s="28">
         <v>157.19999999999999</v>
@@ -4098,20 +4192,20 @@
     </row>
     <row r="13" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B13" s="28">
         <v>26</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D13" s="28">
         <f t="shared" si="0"/>
         <v>11.793415645326633</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F13" s="28">
         <v>173.7</v>
@@ -4123,7 +4217,7 @@
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="47" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B14" s="47"/>
       <c r="C14" s="47"/>
@@ -4134,20 +4228,20 @@
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B15" s="28">
         <v>21.1</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D15" s="28">
         <f>B15/2.20462</f>
         <v>9.5708103890919993</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F15" s="28">
         <v>156.30000000000001</v>
@@ -4159,20 +4253,20 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B16" s="28">
         <v>18.399999999999999</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D16" s="28">
         <f>B16/2.20462</f>
         <v>8.3461095336157705</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F16" s="28">
         <v>152.6</v>
@@ -4183,7 +4277,7 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="47" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B17" s="47"/>
       <c r="C17" s="47"/>
@@ -4194,20 +4288,20 @@
     </row>
     <row r="18" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B18" s="28">
         <v>120.7</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D18" s="28">
         <f>B18/2.20462</f>
         <v>54.748664168881717</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F18" s="28">
         <v>120.6</v>
@@ -4219,20 +4313,20 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B19" s="28">
         <v>32.4</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D19" s="28">
         <f>B19/2.20462</f>
         <v>14.696410265714727</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F19" s="28">
         <v>225.1</v>
@@ -4244,21 +4338,21 @@
     </row>
     <row r="20" spans="1:9" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B20" s="28">
         <f>F20*5.796/42</f>
         <v>22.093800000000002</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D20" s="28">
         <f>B20/2.20462</f>
         <v>10.021591022489138</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F20" s="28">
         <v>160.1</v>
@@ -4270,7 +4364,7 @@
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="47" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B21" s="47"/>
       <c r="C21" s="47"/>
@@ -4281,21 +4375,21 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B22" s="28">
         <f>F22*6.636/42</f>
         <v>26.3386</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D22" s="28">
         <f>B22/2.20462</f>
         <v>11.94700220446154</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F22" s="28">
         <v>166.7</v>
@@ -4307,21 +4401,21 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B23" s="28">
         <f>F23*6.065/42</f>
         <v>23.624619047619049</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D23" s="28">
         <f>B23/2.20462</f>
         <v>10.715959688118158</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F23" s="28">
         <v>163.6</v>
@@ -4333,21 +4427,21 @@
     </row>
     <row r="24" spans="1:9" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B24" s="28">
         <f>F24*6.636/42</f>
         <v>24.742799999999999</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D24" s="28">
         <f>B24/2.20462</f>
         <v>11.223158639584147</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F24" s="28">
         <v>156.6</v>
@@ -4359,21 +4453,21 @@
     </row>
     <row r="25" spans="1:9" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B25" s="28">
         <f>F25*5.248/42</f>
         <v>20.054857142857145</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D25" s="28">
         <f>B25/2.20462</f>
         <v>9.0967409997446946</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F25" s="28">
         <v>160.5</v>
@@ -4385,21 +4479,21 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B26" s="28">
         <f>F26*5.537/42</f>
         <v>21.106516666666668</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D26" s="28">
         <f>B26/2.20462</f>
         <v>9.5737663028851543</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F26" s="28">
         <v>160.1</v>
@@ -4411,7 +4505,7 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="48" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B27" s="48"/>
       <c r="C27" s="48"/>
@@ -4422,20 +4516,20 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B28" s="28">
         <v>5685</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D28" s="28">
         <f>B28/2.20462</f>
         <v>2578.675690141612</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F28" s="28">
         <v>228.6</v>
@@ -4454,20 +4548,20 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B29" s="28">
         <v>4931.3</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D29" s="28">
         <f>B29/2.20462</f>
         <v>2236.8027142999704</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F29" s="28">
         <v>205.7</v>
@@ -4482,20 +4576,20 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B30" s="28">
         <v>3715.9</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D30" s="28">
         <f>B30/2.20462</f>
         <v>1685.5058921718937</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F30" s="28">
         <v>214.3</v>
@@ -4516,14 +4610,14 @@
         <v>2791.6</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D31" s="28">
         <f>B31/2.20462</f>
         <v>1266.2499659805319</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F31" s="28">
         <v>215.4</v>
@@ -4542,21 +4636,21 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B32" s="30">
         <f>F32*24.8</f>
         <v>6239.68</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D32" s="30">
         <f>B32/2.20462</f>
         <v>2830.2746051473728</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F32" s="30">
         <v>251.6</v>
@@ -4568,7 +4662,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B33" s="30"/>
       <c r="C33" s="30"/>
@@ -4579,14 +4673,14 @@
     </row>
     <row r="34" spans="1:7" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C34" s="32"/>
       <c r="D34" s="32" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E34" s="30"/>
       <c r="F34" s="30">
@@ -4599,20 +4693,20 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B35" s="30">
         <v>5771</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D35" s="30">
         <f>B35/2.20462</f>
         <v>2617.6846803530771</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F35" s="30">
         <v>91.9</v>
@@ -4624,20 +4718,20 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B36" s="30">
         <v>6160</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D36" s="30">
         <f>B36/2.20462</f>
         <v>2794.1323221235407</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F36" s="30">
         <v>189.54</v>
@@ -4649,21 +4743,21 @@
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B37" s="33">
         <f>F37*4.4</f>
         <v>924.00000000000011</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D37" s="30">
         <f>B37/2.20462</f>
         <v>419.11984831853118</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F37" s="34">
         <v>210</v>
@@ -4675,7 +4769,7 @@
     </row>
     <row r="38" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="42" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B38" s="42"/>
       <c r="C38" s="42"/>
@@ -4686,7 +4780,7 @@
     </row>
     <row r="39" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="43" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B39" s="43"/>
       <c r="C39" s="43"/>
@@ -4697,7 +4791,7 @@
     </row>
     <row r="40" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="43" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B40" s="43"/>
       <c r="C40" s="43"/>
@@ -4746,4 +4840,327 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B1" s="53" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="L1" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B2" s="49">
+        <v>2015</v>
+      </c>
+      <c r="C2" s="49">
+        <v>2020</v>
+      </c>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49">
+        <v>2030</v>
+      </c>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49">
+        <v>2040</v>
+      </c>
+      <c r="H2" s="51"/>
+      <c r="I2" s="50">
+        <v>2050</v>
+      </c>
+      <c r="L2" s="49">
+        <v>2015</v>
+      </c>
+      <c r="M2" s="49">
+        <v>2020</v>
+      </c>
+      <c r="N2" s="49">
+        <v>2025</v>
+      </c>
+      <c r="O2" s="49">
+        <v>2030</v>
+      </c>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51">
+        <v>2040</v>
+      </c>
+      <c r="R2" s="51"/>
+      <c r="S2" s="50">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="52">
+        <v>1.08</v>
+      </c>
+      <c r="C3" s="52">
+        <v>0.42338626119115846</v>
+      </c>
+      <c r="D3" s="52">
+        <f>AVERAGE(C3,E3)</f>
+        <v>0.36220985917529025</v>
+      </c>
+      <c r="E3" s="52">
+        <v>0.30103345715942204</v>
+      </c>
+      <c r="F3" s="52">
+        <f>AVERAGE(E3,G3)</f>
+        <v>0.28231573196898363</v>
+      </c>
+      <c r="G3" s="52">
+        <v>0.26359800677854528</v>
+      </c>
+      <c r="H3" s="52">
+        <f>AVERAGE(G3,I3)</f>
+        <v>0.25244509003429821</v>
+      </c>
+      <c r="I3" s="52">
+        <v>0.24129217329005115</v>
+      </c>
+      <c r="K3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L3" s="55">
+        <v>1.5007999999999999</v>
+      </c>
+      <c r="M3" s="55">
+        <v>1.07</v>
+      </c>
+      <c r="N3" s="52">
+        <f>AVERAGE(M3,O3)</f>
+        <v>0.94902744482589196</v>
+      </c>
+      <c r="O3" s="55">
+        <v>0.82805488965178387</v>
+      </c>
+      <c r="P3" s="52">
+        <f>AVERAGE(O3,Q3)</f>
+        <v>0.76092108622983057</v>
+      </c>
+      <c r="Q3" s="52">
+        <f>AVERAGE(O3,S3)</f>
+        <v>0.69378728280787727</v>
+      </c>
+      <c r="R3" s="52">
+        <f>AVERAGE(Q3,S3)</f>
+        <v>0.62665347938592397</v>
+      </c>
+      <c r="S3" s="55">
+        <v>0.55951967596397068</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>9500</v>
+      </c>
+      <c r="C4">
+        <v>7000</v>
+      </c>
+      <c r="E4">
+        <v>5800</v>
+      </c>
+      <c r="G4">
+        <v>5300</v>
+      </c>
+      <c r="I4">
+        <v>5000</v>
+      </c>
+      <c r="K4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="54">
+        <v>15000</v>
+      </c>
+      <c r="M4" s="54">
+        <v>12800</v>
+      </c>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54">
+        <v>10300</v>
+      </c>
+      <c r="P4" s="58"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="54">
+        <v>8700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="59">
+        <f>B4/(B3*1000000)</f>
+        <v>8.7962962962962968E-3</v>
+      </c>
+      <c r="C5" s="59">
+        <f t="shared" ref="C5:G5" si="0">C4/(C3*1000000)</f>
+        <v>1.6533365963047882E-2</v>
+      </c>
+      <c r="D5" s="59">
+        <f>AVERAGE(C5,E5)</f>
+        <v>1.7900163682854128E-2</v>
+      </c>
+      <c r="E5" s="59">
+        <f t="shared" si="0"/>
+        <v>1.9266961402660373E-2</v>
+      </c>
+      <c r="F5" s="59">
+        <f>AVERAGE(E5,G5)</f>
+        <v>1.9686667492785428E-2</v>
+      </c>
+      <c r="G5" s="59">
+        <f t="shared" si="0"/>
+        <v>2.0106373582910481E-2</v>
+      </c>
+      <c r="H5" s="59">
+        <f>AVERAGE(G5,I5)</f>
+        <v>2.0414069889784392E-2</v>
+      </c>
+      <c r="I5" s="59">
+        <f>I4/(I3*1000000)</f>
+        <v>2.0721766196658307E-2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>144</v>
+      </c>
+      <c r="L5" s="59">
+        <f>L4/(L3*1000000)</f>
+        <v>9.9946695095948831E-3</v>
+      </c>
+      <c r="M5" s="59">
+        <f>M4/(M3*1000000)</f>
+        <v>1.1962616822429906E-2</v>
+      </c>
+      <c r="N5" s="59">
+        <f>AVERAGE(M5,O5)</f>
+        <v>1.2200702879334927E-2</v>
+      </c>
+      <c r="O5" s="59">
+        <f>O4/(O3*1000000)</f>
+        <v>1.2438788936239948E-2</v>
+      </c>
+      <c r="P5" s="59">
+        <f>AVERAGE(O5,Q5)</f>
+        <v>1.3216354462426583E-2</v>
+      </c>
+      <c r="Q5" s="59">
+        <f>AVERAGE(O5,S5)</f>
+        <v>1.3993919988613216E-2</v>
+      </c>
+      <c r="R5" s="59">
+        <f>AVERAGE(Q5,S5)</f>
+        <v>1.4771485514799851E-2</v>
+      </c>
+      <c r="S5" s="59">
+        <f>S4/(S3*1000000)</f>
+        <v>1.5549051040986486E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <f>AVERAGE(C6,E6)</f>
+        <v>37.5</v>
+      </c>
+      <c r="E6">
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <f>AVERAGE(E6,G6)</f>
+        <v>40</v>
+      </c>
+      <c r="G6">
+        <v>40</v>
+      </c>
+      <c r="H6">
+        <f>AVERAGE(G6,I6)</f>
+        <v>40</v>
+      </c>
+      <c r="I6">
+        <v>40</v>
+      </c>
+      <c r="K6" t="s">
+        <v>119</v>
+      </c>
+      <c r="L6" s="56">
+        <v>30</v>
+      </c>
+      <c r="M6" s="56">
+        <v>35</v>
+      </c>
+      <c r="N6">
+        <f>AVERAGE(M6,O6)</f>
+        <v>37.5</v>
+      </c>
+      <c r="O6" s="56">
+        <v>40</v>
+      </c>
+      <c r="P6">
+        <f>AVERAGE(O6,Q6)</f>
+        <v>40</v>
+      </c>
+      <c r="Q6" s="57">
+        <f>AVERAGE(O6,S6)</f>
+        <v>40</v>
+      </c>
+      <c r="R6">
+        <f>AVERAGE(Q6,S6)</f>
+        <v>40</v>
+      </c>
+      <c r="S6" s="56">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="L1:S1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>